<commit_message>
First version of assign Device to Identity
</commit_message>
<xml_diff>
--- a/ToDelete/ODS_Beschrijving_SalesManagement_AFC_R3.xlsx
+++ b/ToDelete/ODS_Beschrijving_SalesManagement_AFC_R3.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CMDB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CMDB\ToDelete\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,12 +33,12 @@
     <sheet name="lov_15" sheetId="18" state="hidden" r:id="rId19"/>
     <sheet name="lov_16" sheetId="19" state="hidden" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="613">
   <si>
     <t>oracle.dbtools.crest.model.design.relational.Table</t>
   </si>
@@ -1800,6 +1800,84 @@
   </si>
   <si>
     <t>CODE_NAMES</t>
+  </si>
+  <si>
+    <t>RAW(16)</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>VARCHAR2(200 CHAR)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(255 CHAR)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(512 CHAR)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(50 CHAR)</t>
+  </si>
+  <si>
+    <t>NUMBER(10,0)</t>
+  </si>
+  <si>
+    <t>REJECTED_CODE</t>
+  </si>
+  <si>
+    <t>ERROR_CODE</t>
+  </si>
+  <si>
+    <t>REJECTED_REASON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARCHAR2(512 CHAR)          </t>
+  </si>
+  <si>
+    <t>ERROR_REDEN</t>
+  </si>
+  <si>
+    <t>NCLOB</t>
+  </si>
+  <si>
+    <t>NVARCHAR2(50)</t>
+  </si>
+  <si>
+    <t>NVARCHAR2(100)</t>
+  </si>
+  <si>
+    <t>NUMBER(2,0)</t>
+  </si>
+  <si>
+    <t>NUMBER(18,2)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(100 CHAR)</t>
+  </si>
+  <si>
+    <t>NUMBER(1,0)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(20 CHAR)</t>
+  </si>
+  <si>
+    <t>AS400_ID</t>
+  </si>
+  <si>
+    <t>VARCHAR2(500 CHAR)</t>
+  </si>
+  <si>
+    <t>INTERVAL DAY(2) TO SECOND(6)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(64 CHAR)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(10 CHAR)</t>
+  </si>
+  <si>
+    <t>NUMBER(10,2)</t>
   </si>
 </sst>
 </file>
@@ -1868,7 +1946,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1889,26 +1967,6 @@
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1943,6 +2001,47 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="8"/>
       </left>
       <right style="thin">
@@ -1951,16 +2050,38 @@
       <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
-      </bottom>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1977,25 +2098,17 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2009,8 +2122,31 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2020,7 +2156,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2052,7 +2188,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="kapsch_CMYK_71mm_blackyellow_300dpi"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="kapsch_CMYK_71mm_blackyellow_300dpi">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2125,7 +2267,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1192" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="1192" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000A8040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2170,9 +2318,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2210,7 +2358,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2316,7 +2464,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4129,1808 +4277,2446 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D226"/>
+  <dimension ref="A2:F227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="A148" sqref="A148:B148"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C8:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="30.6640625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="2"/>
+    <col min="5" max="5" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="15"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="17"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="C9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
-      <c r="C10" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C10" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>502</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
-      <c r="C11" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C11" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
-      <c r="C12" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C12" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>504</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
-      <c r="C13" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C13" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
-      <c r="C14" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C14" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>591</v>
+      </c>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-      <c r="C15" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C15" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>505</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
-      <c r="C16" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C16" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>591</v>
+      </c>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
-      <c r="C17" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C17" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
-      <c r="C18" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="F18" s="16"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
-      <c r="C19" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>506</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
-      <c r="C20" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C20" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>594</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="F20" s="16"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="15"/>
+      <c r="C21" s="10" t="s">
+        <v>598</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>596</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>597</v>
+      </c>
+      <c r="F21" s="16"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="C24" s="13"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
-      <c r="C27" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="C28" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="F28" s="16"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="C29" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>571</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F29" s="16"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="C30" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>508</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F30" s="16"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="C31" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="C32" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>509</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>591</v>
+      </c>
+      <c r="F32" s="16"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="C33" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="3"/>
+      <c r="C34" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D34" s="14" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="15"/>
+      <c r="E34" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B37" s="6" t="s">
         <v>510</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+      <c r="C37" s="13"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
-      <c r="C40" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="C41" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="F41" s="16"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="C42" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>599</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="C43" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="F43" s="16"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="C44" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>504</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>599</v>
+      </c>
+      <c r="F44" s="16"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="C45" s="6" t="s">
-        <v>575</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F45" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="C46" s="6" t="s">
-        <v>576</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+        <v>575</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>600</v>
+      </c>
+      <c r="F46" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="C47" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+        <v>576</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>601</v>
+      </c>
+      <c r="F47" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="C48" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>509</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>591</v>
+      </c>
+      <c r="F48" s="16"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="C49" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>511</v>
+      </c>
+      <c r="F49" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="C50" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="3"/>
+      <c r="C51" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="D51" s="14" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="15"/>
+      <c r="E51" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="F51" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B54" s="6" t="s">
         <v>586</v>
       </c>
-      <c r="C53" s="16"/>
-      <c r="D53" s="3"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="3"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
+      <c r="C54" s="13"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
-      <c r="C56" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="C57" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="F57" s="16"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="C58" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E58" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F58" s="16"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="C59" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D59" s="14" t="s">
+        <v>512</v>
+      </c>
+      <c r="E59" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F59" s="16"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="3"/>
+      <c r="C60" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D60" s="14" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="15"/>
+      <c r="E60" s="16" t="s">
+        <v>602</v>
+      </c>
+      <c r="F60" s="16"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="6" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B63" s="6" t="s">
         <v>513</v>
       </c>
-      <c r="C62" s="16"/>
-      <c r="D62" s="3"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
+      <c r="C63" s="13"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
-      <c r="C66" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="C67" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>514</v>
+      </c>
+      <c r="E67" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F67" s="16"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="C68" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>515</v>
+      </c>
+      <c r="E68" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="F68" s="16"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="C69" s="6" t="s">
-        <v>572</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>516</v>
+      </c>
+      <c r="E69" s="16" t="s">
+        <v>604</v>
+      </c>
+      <c r="F69" s="16"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="C70" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+        <v>572</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E70" s="16" t="s">
+        <v>604</v>
+      </c>
+      <c r="F70" s="16"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
       <c r="C71" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>517</v>
+      </c>
+      <c r="E71" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="F71" s="16"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
       <c r="C72" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E72" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F72" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="3"/>
       <c r="C73" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E73" s="16" t="s">
+        <v>605</v>
+      </c>
+      <c r="F73" s="16"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="3"/>
       <c r="C74" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>518</v>
+      </c>
+      <c r="E74" s="16" t="s">
+        <v>604</v>
+      </c>
+      <c r="F74" s="16"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
       <c r="C75" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="E75" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="F75" s="16"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="3"/>
       <c r="C76" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>519</v>
+      </c>
+      <c r="E76" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="F76" s="16"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="3"/>
       <c r="C77" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="E77" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F77" s="16"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="C78" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>520</v>
+      </c>
+      <c r="E78" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F78" s="16"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="3"/>
       <c r="C79" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+      <c r="D79" s="14" t="s">
+        <v>521</v>
+      </c>
+      <c r="E79" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F79" s="16"/>
+    </row>
+    <row r="80" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="C80" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>522</v>
+      </c>
+      <c r="E80" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F80" s="16"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
       <c r="C81" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>523</v>
+      </c>
+      <c r="E81" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="F81" s="16"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="3"/>
       <c r="C82" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>524</v>
+      </c>
+      <c r="E82" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="F82" s="16"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="3"/>
       <c r="C83" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="D83" s="6" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>525</v>
+      </c>
+      <c r="E83" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="F83" s="16"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="3"/>
       <c r="C84" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>526</v>
+      </c>
+      <c r="E84" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="F84" s="16"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="3"/>
       <c r="C85" s="6" t="s">
-        <v>577</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="E85" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F85" s="16"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="3"/>
       <c r="C86" s="6" t="s">
-        <v>578</v>
-      </c>
-      <c r="D86" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+        <v>577</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E86" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="F86" s="16"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="3"/>
       <c r="C87" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="E87" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F87" s="16"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="3"/>
+      <c r="C88" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="D87" s="6" t="s">
+      <c r="D88" s="14" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F88" s="16"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" s="5"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="15"/>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
       <c r="D90" s="3"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="6" t="s">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="3"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B91" s="6" t="s">
+      <c r="B92" s="6" t="s">
         <v>528</v>
       </c>
-      <c r="C91" s="16"/>
-      <c r="D91" s="3"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" s="3"/>
-      <c r="B92" s="3"/>
-      <c r="C92" s="3"/>
+      <c r="C92" s="13"/>
       <c r="D92" s="3"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="3"/>
-      <c r="B93" s="14"/>
-      <c r="C93" s="14"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
       <c r="D93" s="3"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="3"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B94" s="11"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="3"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="3"/>
-      <c r="C95" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D95" s="6" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C95" s="8"/>
+      <c r="D95" s="8"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="3"/>
       <c r="C96" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D96" s="6" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="D96" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="E96" s="16" t="s">
+        <v>606</v>
+      </c>
+      <c r="F96" s="16"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="3"/>
       <c r="C97" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="D97" s="14" t="s">
+        <v>530</v>
+      </c>
+      <c r="E97" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="F97" s="16"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="3"/>
       <c r="C98" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D98" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="D98" s="14" t="s">
+        <v>511</v>
+      </c>
+      <c r="E98" s="16" t="s">
+        <v>606</v>
+      </c>
+      <c r="F98" s="16"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="3"/>
       <c r="C99" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D99" s="6" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="D99" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E99" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F99" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="3"/>
       <c r="C100" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="D100" s="6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="D100" s="14" t="s">
+        <v>531</v>
+      </c>
+      <c r="E100" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="F100" s="16"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="3"/>
       <c r="C101" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D101" s="6" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="E101" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="F101" s="16"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="3"/>
       <c r="C102" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D102" s="14" t="s">
+        <v>532</v>
+      </c>
+      <c r="E102" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F102" s="16"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="3"/>
+      <c r="C103" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="D102" s="6" t="s">
+      <c r="D103" s="14" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" s="3"/>
-      <c r="B103" s="3"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" s="5"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="15"/>
+      <c r="E103" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="F103" s="16"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="3"/>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
       <c r="D104" s="3"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" s="6" t="s">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="5"/>
+      <c r="B105" s="5"/>
+      <c r="C105" s="12"/>
+      <c r="D105" s="3"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B105" s="6" t="s">
+      <c r="B106" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="C105" s="16"/>
-      <c r="D105" s="3"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" s="3"/>
-      <c r="B106" s="3"/>
-      <c r="C106" s="3"/>
+      <c r="C106" s="13"/>
       <c r="D106" s="3"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="3"/>
-      <c r="B107" s="14"/>
-      <c r="C107" s="14"/>
+      <c r="B107" s="3"/>
+      <c r="C107" s="3"/>
       <c r="D107" s="3"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="3"/>
-      <c r="C108" s="10"/>
-      <c r="D108" s="10"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B108" s="11"/>
+      <c r="C108" s="11"/>
+      <c r="D108" s="3"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="3"/>
-      <c r="C109" s="6" t="s">
-        <v>535</v>
-      </c>
-      <c r="D109" s="6" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C109" s="8"/>
+      <c r="D109" s="8"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="3"/>
       <c r="C110" s="6" t="s">
-        <v>536</v>
-      </c>
-      <c r="D110" s="6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+        <v>535</v>
+      </c>
+      <c r="D110" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="E110" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F110" s="16"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="3"/>
       <c r="C111" s="6" t="s">
-        <v>537</v>
-      </c>
-      <c r="D111" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+        <v>536</v>
+      </c>
+      <c r="D111" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E111" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F111" s="16"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="3"/>
       <c r="C112" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D112" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+        <v>537</v>
+      </c>
+      <c r="D112" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E112" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="F112" s="16"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="3"/>
       <c r="C113" s="6" t="s">
-        <v>538</v>
-      </c>
-      <c r="D113" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="D113" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E113" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F113" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="3"/>
       <c r="C114" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="D114" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="E114" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F114" s="16"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="3"/>
+      <c r="C115" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D114" s="6" t="s">
+      <c r="D115" s="14" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A115" s="3"/>
-      <c r="B115" s="3"/>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E115" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F115" s="16"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A118" s="5"/>
-      <c r="B118" s="5"/>
-      <c r="C118" s="15"/>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" s="3"/>
+      <c r="B118" s="3"/>
+      <c r="C118" s="3"/>
       <c r="D118" s="3"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A119" s="6" t="s">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" s="5"/>
+      <c r="B119" s="5"/>
+      <c r="C119" s="12"/>
+      <c r="D119" s="3"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B119" s="6" t="s">
+      <c r="B120" s="6" t="s">
         <v>539</v>
       </c>
-      <c r="C119" s="16"/>
-      <c r="D119" s="3"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A120" s="3"/>
-      <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
+      <c r="C120" s="13"/>
       <c r="D120" s="3"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="3"/>
-      <c r="B121" s="14"/>
-      <c r="C121" s="14"/>
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
       <c r="D121" s="3"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="3"/>
-      <c r="C122" s="10"/>
-      <c r="D122" s="10"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B122" s="11"/>
+      <c r="C122" s="11"/>
+      <c r="D122" s="3"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="3"/>
-      <c r="C123" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D123" s="6" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C123" s="8"/>
+      <c r="D123" s="8"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="3"/>
       <c r="C124" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D124" s="6" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="D124" s="14" t="s">
+        <v>540</v>
+      </c>
+      <c r="E124" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="F124" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="3"/>
       <c r="C125" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D125" s="6" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="D125" s="14" t="s">
+        <v>502</v>
+      </c>
+      <c r="E125" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="F125" s="16"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="3"/>
       <c r="C126" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D126" s="6" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="D126" s="14" t="s">
+        <v>541</v>
+      </c>
+      <c r="E126" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F126" s="16"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="3"/>
       <c r="C127" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D127" s="6" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="D127" s="14" t="s">
+        <v>542</v>
+      </c>
+      <c r="E127" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F127" s="16"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="3"/>
       <c r="C128" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D128" s="6" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+      <c r="D128" s="14" t="s">
+        <v>543</v>
+      </c>
+      <c r="E128" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="F128" s="16"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="3"/>
       <c r="C129" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D129" s="6" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+      <c r="D129" s="14" t="s">
+        <v>544</v>
+      </c>
+      <c r="E129" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="F129" s="16"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="3"/>
       <c r="C130" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D130" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="D130" s="14" t="s">
+        <v>545</v>
+      </c>
+      <c r="E130" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="F130" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="3"/>
       <c r="C131" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="D131" s="6" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="D131" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E131" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F131" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="3"/>
       <c r="C132" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="D132" s="6" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+      <c r="D132" s="14" t="s">
+        <v>546</v>
+      </c>
+      <c r="E132" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="F132" s="16"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="3"/>
       <c r="C133" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="D133" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="D133" s="14" t="s">
+        <v>547</v>
+      </c>
+      <c r="E133" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F133" s="16"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="3"/>
       <c r="C134" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D134" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E134" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F134" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" s="3"/>
+      <c r="C135" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="D134" s="6" t="s">
+      <c r="D135" s="18" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A135" s="3"/>
-      <c r="C135" s="6" t="s">
+      <c r="E135" s="19" t="s">
+        <v>593</v>
+      </c>
+      <c r="F135" s="19"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" s="3"/>
+      <c r="C136" s="20" t="s">
         <v>269</v>
       </c>
-      <c r="D135" s="6" t="s">
+      <c r="D136" s="20" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A136" s="3"/>
-      <c r="B136" s="3"/>
-      <c r="C136" s="3"/>
-      <c r="D136" s="3"/>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E136" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="F136" s="16"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
-      <c r="C137" s="3"/>
-      <c r="D137" s="3"/>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C137" s="21" t="s">
+        <v>607</v>
+      </c>
+      <c r="D137" s="21" t="s">
+        <v>607</v>
+      </c>
+      <c r="E137" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="F137" s="16"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
       <c r="D138" s="3"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A139" s="5"/>
-      <c r="B139" s="5"/>
-      <c r="C139" s="15"/>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" s="3"/>
+      <c r="B139" s="3"/>
+      <c r="C139" s="3"/>
       <c r="D139" s="3"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A140" s="6" t="s">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" s="5"/>
+      <c r="B140" s="5"/>
+      <c r="C140" s="12"/>
+      <c r="D140" s="3"/>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B140" s="6" t="s">
+      <c r="B141" s="6" t="s">
         <v>549</v>
       </c>
-      <c r="C140" s="16"/>
-      <c r="D140" s="3"/>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A141" s="3"/>
-      <c r="B141" s="3"/>
-      <c r="C141" s="3"/>
+      <c r="C141" s="13"/>
       <c r="D141" s="3"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="3"/>
-      <c r="B142" s="14"/>
-      <c r="C142" s="14"/>
+      <c r="B142" s="3"/>
+      <c r="C142" s="3"/>
       <c r="D142" s="3"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="3"/>
-      <c r="C143" s="10"/>
-      <c r="D143" s="10"/>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B143" s="11"/>
+      <c r="C143" s="11"/>
+      <c r="D143" s="3"/>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="3"/>
-      <c r="C144" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D144" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C144" s="8"/>
+      <c r="D144" s="8"/>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="3"/>
       <c r="C145" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D145" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="D145" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E145" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="F145" s="16"/>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" s="3"/>
       <c r="C146" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D146" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E146" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F146" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A147" s="3"/>
+      <c r="C147" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="D146" s="6" t="s">
+      <c r="D147" s="14" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A147" s="3"/>
-      <c r="B147" s="3"/>
-      <c r="C147" s="3"/>
-      <c r="D147" s="3"/>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A148" s="5"/>
-      <c r="B148" s="5"/>
-      <c r="C148" s="15"/>
+      <c r="E147" s="16" t="s">
+        <v>608</v>
+      </c>
+      <c r="F147" s="16"/>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A148" s="3"/>
+      <c r="B148" s="3"/>
+      <c r="C148" s="3"/>
       <c r="D148" s="3"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A149" s="6" t="s">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A149" s="5"/>
+      <c r="B149" s="5"/>
+      <c r="C149" s="12"/>
+      <c r="D149" s="3"/>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A150" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B149" s="6" t="s">
+      <c r="B150" s="6" t="s">
         <v>550</v>
       </c>
-      <c r="C149" s="16"/>
-      <c r="D149" s="3"/>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A150" s="3"/>
-      <c r="B150" s="3"/>
-      <c r="C150" s="3"/>
+      <c r="C150" s="13"/>
       <c r="D150" s="3"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="3"/>
-      <c r="B151" s="14"/>
-      <c r="C151" s="14"/>
+      <c r="B151" s="3"/>
+      <c r="C151" s="3"/>
       <c r="D151" s="3"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="3"/>
-      <c r="C152" s="10"/>
-      <c r="D152" s="10"/>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B152" s="11"/>
+      <c r="C152" s="11"/>
+      <c r="D152" s="3"/>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="3"/>
-      <c r="C153" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D153" s="6" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C153" s="8"/>
+      <c r="D153" s="8"/>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="3"/>
       <c r="C154" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D154" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="D154" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="E154" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="F154" s="16"/>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="3"/>
       <c r="C155" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D155" s="6" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="D155" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E155" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F155" s="16"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="3"/>
       <c r="C156" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D156" s="6" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="D156" s="14" t="s">
+        <v>551</v>
+      </c>
+      <c r="E156" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F156" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="3"/>
       <c r="C157" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D157" s="6" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="D157" s="14" t="s">
+        <v>552</v>
+      </c>
+      <c r="E157" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="F157" s="16"/>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="3"/>
       <c r="C158" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D158" s="6" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="D158" s="14" t="s">
+        <v>553</v>
+      </c>
+      <c r="E158" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F158" s="16"/>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="3"/>
       <c r="C159" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D159" s="6" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="D159" s="14" t="s">
+        <v>554</v>
+      </c>
+      <c r="E159" s="16" t="s">
+        <v>609</v>
+      </c>
+      <c r="F159" s="16"/>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="3"/>
       <c r="C160" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D160" s="6" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="D160" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="E160" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="F160" s="16"/>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="3"/>
       <c r="C161" s="6" t="s">
-        <v>582</v>
-      </c>
-      <c r="D161" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="D161" s="14" t="s">
+        <v>504</v>
+      </c>
+      <c r="E161" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F161" s="16"/>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="3"/>
       <c r="C162" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D162" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+        <v>582</v>
+      </c>
+      <c r="D162" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E162" s="16" t="s">
+        <v>605</v>
+      </c>
+      <c r="F162" s="16"/>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="3"/>
       <c r="C163" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="D163" s="6" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="D163" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E163" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F163" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="3"/>
       <c r="C164" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D164" s="6" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+      <c r="D164" s="14" t="s">
+        <v>555</v>
+      </c>
+      <c r="E164" s="16" t="s">
+        <v>605</v>
+      </c>
+      <c r="F164" s="16"/>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="3"/>
       <c r="C165" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="D165" s="6" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="D165" s="14" t="s">
+        <v>556</v>
+      </c>
+      <c r="E165" s="16" t="s">
+        <v>605</v>
+      </c>
+      <c r="F165" s="16"/>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="3"/>
       <c r="C166" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="D166" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="D166" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="E166" s="16" t="s">
+        <v>605</v>
+      </c>
+      <c r="F166" s="16"/>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="3"/>
       <c r="C167" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="D167" s="6" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="D167" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E167" s="16" t="s">
+        <v>511</v>
+      </c>
+      <c r="F167" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="3"/>
       <c r="C168" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="D168" s="6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+      <c r="D168" s="14" t="s">
+        <v>558</v>
+      </c>
+      <c r="E168" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F168" s="16"/>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="3"/>
       <c r="C169" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="D169" s="6" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+      <c r="D169" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="E169" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="F169" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="3"/>
       <c r="C170" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="D170" s="6" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+      <c r="D170" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="E170" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="F170" s="16"/>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="3"/>
       <c r="C171" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D171" s="6" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+      <c r="D171" s="14" t="s">
+        <v>560</v>
+      </c>
+      <c r="E171" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="F171" s="16"/>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="3"/>
       <c r="C172" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="D172" s="6" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+      <c r="D172" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="E172" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F172" s="16"/>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" s="3"/>
       <c r="C173" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="D173" s="6" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+      <c r="D173" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="E173" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="F173" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" s="3"/>
       <c r="C174" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="D174" s="6" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+      <c r="D174" s="14" t="s">
+        <v>548</v>
+      </c>
+      <c r="E174" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="F174" s="16"/>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" s="3"/>
       <c r="C175" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="D175" s="6" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+      <c r="D175" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="E175" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="F175" s="16"/>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" s="3"/>
       <c r="C176" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="D176" s="6" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+      <c r="D176" s="14" t="s">
+        <v>562</v>
+      </c>
+      <c r="E176" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="F176" s="16"/>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" s="3"/>
       <c r="C177" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="D177" s="6" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+      <c r="D177" s="14" t="s">
+        <v>563</v>
+      </c>
+      <c r="E177" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="F177" s="16"/>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" s="3"/>
       <c r="C178" s="6" t="s">
-        <v>579</v>
-      </c>
-      <c r="D178" s="6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+      <c r="D178" s="14" t="s">
+        <v>564</v>
+      </c>
+      <c r="E178" s="16" t="s">
+        <v>611</v>
+      </c>
+      <c r="F178" s="16"/>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" s="3"/>
       <c r="C179" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="D179" s="6" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+        <v>579</v>
+      </c>
+      <c r="D179" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E179" s="16" t="s">
+        <v>610</v>
+      </c>
+      <c r="F179" s="16"/>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" s="3"/>
       <c r="C180" s="6" t="s">
-        <v>580</v>
-      </c>
-      <c r="D180" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+        <v>265</v>
+      </c>
+      <c r="D180" s="14" t="s">
+        <v>565</v>
+      </c>
+      <c r="E180" s="16" t="s">
+        <v>610</v>
+      </c>
+      <c r="F180" s="16"/>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" s="3"/>
       <c r="C181" s="6" t="s">
+        <v>580</v>
+      </c>
+      <c r="D181" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E181" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="F181" s="16"/>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A182" s="3"/>
+      <c r="C182" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="D181" s="6" t="s">
+      <c r="D182" s="14" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A182" s="3"/>
-      <c r="B182" s="3"/>
-      <c r="C182" s="3"/>
-      <c r="D182" s="3"/>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E182" s="16" t="s">
+        <v>605</v>
+      </c>
+      <c r="F182" s="16"/>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="3"/>
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
       <c r="D183" s="3"/>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" s="3"/>
       <c r="B184" s="3"/>
       <c r="C184" s="3"/>
       <c r="D184" s="3"/>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A185" s="5"/>
-      <c r="B185" s="5"/>
-      <c r="C185" s="15"/>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A185" s="3"/>
+      <c r="B185" s="3"/>
+      <c r="C185" s="3"/>
       <c r="D185" s="3"/>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A186" s="6" t="s">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A186" s="5"/>
+      <c r="B186" s="5"/>
+      <c r="C186" s="12"/>
+      <c r="D186" s="3"/>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A187" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B186" s="6" t="s">
+      <c r="B187" s="6" t="s">
         <v>567</v>
       </c>
-      <c r="C186" s="16"/>
-      <c r="D186" s="3"/>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A187" s="3"/>
-      <c r="B187" s="3"/>
-      <c r="C187" s="3"/>
+      <c r="C187" s="13"/>
       <c r="D187" s="3"/>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" s="3"/>
-      <c r="B188" s="14"/>
-      <c r="C188" s="14"/>
+      <c r="B188" s="3"/>
+      <c r="C188" s="3"/>
       <c r="D188" s="3"/>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" s="3"/>
-      <c r="C189" s="10"/>
-      <c r="D189" s="10"/>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B189" s="11"/>
+      <c r="C189" s="11"/>
+      <c r="D189" s="3"/>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" s="3"/>
-      <c r="C190" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D190" s="6" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C190" s="8"/>
+      <c r="D190" s="8"/>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" s="3"/>
       <c r="C191" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D191" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="D191" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="E191" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="F191" s="16"/>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" s="3"/>
       <c r="C192" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D192" s="6" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="D192" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E192" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F192" s="16"/>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" s="3"/>
       <c r="C193" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D193" s="6" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="D193" s="14" t="s">
+        <v>514</v>
+      </c>
+      <c r="E193" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F193" s="16"/>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" s="3"/>
       <c r="C194" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D194" s="6" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="D194" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="E194" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="F194" s="16"/>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" s="3"/>
       <c r="C195" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D195" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="D195" s="14" t="s">
+        <v>504</v>
+      </c>
+      <c r="E195" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F195" s="16"/>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" s="3"/>
       <c r="C196" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="D196" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="D196" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E196" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F196" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" s="3"/>
       <c r="C197" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D197" s="6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="D197" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E197" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="F197" s="16"/>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" s="3"/>
       <c r="C198" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D198" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="E198" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F198" s="16"/>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A199" s="3"/>
+      <c r="C199" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="D198" s="6" t="s">
+      <c r="D199" s="14" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A199" s="3"/>
-      <c r="B199" s="3"/>
-      <c r="C199" s="3"/>
-      <c r="D199" s="3"/>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E199" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F199" s="16"/>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" s="3"/>
       <c r="B200" s="3"/>
       <c r="C200" s="3"/>
       <c r="D200" s="3"/>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" s="3"/>
       <c r="B201" s="3"/>
       <c r="C201" s="3"/>
       <c r="D201" s="3"/>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A202" s="5"/>
-      <c r="B202" s="5"/>
-      <c r="C202" s="15"/>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A202" s="3"/>
+      <c r="B202" s="3"/>
+      <c r="C202" s="3"/>
       <c r="D202" s="3"/>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A203" s="6" t="s">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A203" s="5"/>
+      <c r="B203" s="5"/>
+      <c r="C203" s="12"/>
+      <c r="D203" s="3"/>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A204" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B203" s="6" t="s">
+      <c r="B204" s="6" t="s">
         <v>569</v>
       </c>
-      <c r="C203" s="16"/>
-      <c r="D203" s="3"/>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A204" s="3"/>
-      <c r="B204" s="3"/>
-      <c r="C204" s="3"/>
+      <c r="C204" s="13"/>
       <c r="D204" s="3"/>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" s="3"/>
-      <c r="B205" s="14"/>
-      <c r="C205" s="14"/>
+      <c r="B205" s="3"/>
+      <c r="C205" s="3"/>
       <c r="D205" s="3"/>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" s="3"/>
-      <c r="C206" s="10"/>
-      <c r="D206" s="10"/>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B206" s="11"/>
+      <c r="C206" s="11"/>
+      <c r="D206" s="3"/>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" s="3"/>
-      <c r="C207" s="6" t="s">
+      <c r="C207" s="22"/>
+      <c r="D207" s="22"/>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A208" s="3"/>
+      <c r="C208" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D207" s="6" t="s">
+      <c r="D208" s="20" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A208" s="3"/>
-      <c r="C208" s="6" t="s">
+      <c r="E208" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="F208" s="16"/>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A209" s="3"/>
+      <c r="C209" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D208" s="6" t="s">
+      <c r="D209" s="20" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A209" s="3"/>
-      <c r="C209" s="6" t="s">
+      <c r="E209" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F209" s="16"/>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A210" s="3"/>
+      <c r="C210" s="20" t="s">
         <v>581</v>
       </c>
-      <c r="D209" s="6" t="s">
+      <c r="D210" s="20" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A210" s="3"/>
-      <c r="C210" s="6" t="s">
+      <c r="E210" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="F210" s="16"/>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A211" s="3"/>
+      <c r="C211" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="D210" s="6" t="s">
+      <c r="D211" s="20" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A211" s="3"/>
-      <c r="C211" s="6" t="s">
+      <c r="E211" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="F211" s="16"/>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A212" s="3"/>
+      <c r="C212" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="D211" s="6" t="s">
+      <c r="D212" s="20" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A212" s="3"/>
-      <c r="C212" s="6" t="s">
+      <c r="E212" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F212" s="16"/>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A213" s="3"/>
+      <c r="C213" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="D212" s="6" t="s">
+      <c r="D213" s="20" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A213" s="3"/>
-      <c r="C213" s="6" t="s">
+      <c r="E213" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F213" s="16" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A214" s="3"/>
+      <c r="C214" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="D213" s="6" t="s">
+      <c r="D214" s="20" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A214" s="3"/>
-      <c r="C214" s="6" t="s">
+      <c r="E214" s="16" t="s">
+        <v>612</v>
+      </c>
+      <c r="F214" s="16"/>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A215" s="3"/>
+      <c r="C215" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="D214" s="6" t="s">
+      <c r="D215" s="20" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A215" s="3"/>
-      <c r="C215" s="6" t="s">
+      <c r="E215" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="F215" s="16"/>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A216" s="3"/>
+      <c r="C216" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="D215" s="6" t="s">
+      <c r="D216" s="20" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A216" s="3"/>
-      <c r="C216" s="6" t="s">
+      <c r="E216" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="F216" s="16"/>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A217" s="3"/>
+      <c r="C217" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="D216" s="6" t="s">
+      <c r="D217" s="20" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A217" s="3"/>
-      <c r="C217" s="6" t="s">
+      <c r="E217" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="F217" s="16"/>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A218" s="3"/>
+      <c r="C218" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="D217" s="6" t="s">
+      <c r="D218" s="20" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A218" s="3"/>
-      <c r="C218" s="6" t="s">
+      <c r="E218" s="16" t="s">
+        <v>612</v>
+      </c>
+      <c r="F218" s="16"/>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A219" s="3"/>
+      <c r="C219" s="20" t="s">
         <v>257</v>
       </c>
-      <c r="D218" s="6" t="s">
+      <c r="D219" s="20" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A219" s="3"/>
-      <c r="B219" s="3"/>
-      <c r="C219" s="3"/>
-      <c r="D219" s="3"/>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A220" s="5"/>
-      <c r="B220" s="5"/>
-      <c r="C220" s="3"/>
-      <c r="D220" s="3"/>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A221" s="6" t="s">
-        <v>584</v>
-      </c>
-      <c r="B221" s="6" t="s">
-        <v>585</v>
-      </c>
-      <c r="C221" s="3"/>
-      <c r="D221" s="3"/>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A222" s="3"/>
-      <c r="B222" s="3"/>
-      <c r="C222" s="3"/>
-      <c r="D222" s="3"/>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E219" s="16" t="s">
+        <v>611</v>
+      </c>
+      <c r="F219" s="16"/>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A220" s="3"/>
+      <c r="B220" s="3"/>
+      <c r="C220" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="D220" s="14" t="s">
+        <v>565</v>
+      </c>
+      <c r="E220" s="16" t="s">
+        <v>610</v>
+      </c>
+      <c r="F220" s="16"/>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C221" s="20" t="s">
+        <v>579</v>
+      </c>
+      <c r="D221" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E221" s="16" t="s">
+        <v>610</v>
+      </c>
+      <c r="F221" s="16"/>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C222" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="D222" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E222" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="F222" s="16"/>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" s="3"/>
       <c r="B223" s="3"/>
       <c r="C223" s="3"/>
       <c r="D223" s="3"/>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A224" s="3"/>
-      <c r="B224" s="3"/>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A224" s="5"/>
+      <c r="B224" s="5"/>
       <c r="C224" s="3"/>
       <c r="D224" s="3"/>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A225" s="3"/>
-      <c r="B225" s="3"/>
+      <c r="A225" s="6" t="s">
+        <v>584</v>
+      </c>
+      <c r="B225" s="6" t="s">
+        <v>585</v>
+      </c>
       <c r="C225" s="3"/>
       <c r="D225" s="3"/>
     </row>
@@ -5939,6 +6725,12 @@
       <c r="B226" s="3"/>
       <c r="C226" s="3"/>
       <c r="D226" s="3"/>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227" s="3"/>
+      <c r="B227" s="3"/>
+      <c r="C227" s="3"/>
+      <c r="D227" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8192,15 +8984,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DA77A1B65DDC7C438174C741BEE1440A" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="556e679499179c82c5585af9859fe872">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a0a82402-f287-468d-a4e2-514652d7b906" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1873a0f4b49697fb0fec6fac4a0ffc71" ns2:_="" ns3:_="">
     <xsd:import namespace="a0a82402-f287-468d-a4e2-514652d7b906"/>
@@ -8356,20 +9139,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <_dlc_DocId xmlns="a0a82402-f287-468d-a4e2-514652d7b906">PMSDOC-298-696</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="a0a82402-f287-468d-a4e2-514652d7b906">
-      <Url>http://sharepoint.prodatamobility.com/software/ReTiBo/Collaboration/_layouts/DocIdRedir.aspx?ID=PMSDOC-298-696</Url>
-      <Description>PMSDOC-298-696</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -8415,15 +9194,20 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3E0D151-2B7D-412A-8989-6C48AC2A5D82}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <_dlc_DocId xmlns="a0a82402-f287-468d-a4e2-514652d7b906">PMSDOC-298-696</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="a0a82402-f287-468d-a4e2-514652d7b906">
+      <Url>http://sharepoint.prodatamobility.com/software/ReTiBo/Collaboration/_layouts/DocIdRedir.aspx?ID=PMSDOC-298-696</Url>
+      <Description>PMSDOC-298-696</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D6ABB8D-6D1F-4189-8B06-99F4D54FA638}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8442,7 +9226,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3E0D151-2B7D-412A-8989-6C48AC2A5D82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E60143-3ADC-4D0B-8E5D-5D4450BC1618}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85CE089B-E621-44D7-95B4-FA38A5FAB4CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8451,12 +9251,4 @@
     <ds:schemaRef ds:uri="a0a82402-f287-468d-a4e2-514652d7b906"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E60143-3ADC-4D0B-8E5D-5D4450BC1618}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>